<commit_message>
Update: Revised CMM_Measurements.xlsx with new data
</commit_message>
<xml_diff>
--- a/CMM_Measurements.xlsx
+++ b/CMM_Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokhanpoyraz\Desktop\Çalışmalar\Concentricity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A341464-323B-40BB-B19C-2B510440B5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422FA99A-6C32-41A6-8723-144D8B3E356A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,30 +41,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Diameter_IC CAP</t>
-  </si>
-  <si>
-    <t>Diameter_IC CAP MIN</t>
-  </si>
-  <si>
-    <t>Diameter_IC CAP MAX</t>
-  </si>
-  <si>
-    <t>Roundness_IC CAP</t>
-  </si>
-  <si>
-    <t>Diameter_DIS CAP</t>
-  </si>
-  <si>
-    <t>Diameter_DIS CAP MIN</t>
-  </si>
-  <si>
-    <t>Diameter_DIS CAP MAX</t>
-  </si>
-  <si>
-    <t>Roundness_DIS CAP</t>
-  </si>
-  <si>
     <t>Concentricity1</t>
   </si>
   <si>
@@ -88,6 +64,30 @@
   </si>
   <si>
     <t>Normalized Concentricity</t>
+  </si>
+  <si>
+    <t>Diameter_Inner MIN</t>
+  </si>
+  <si>
+    <t>Diameter_Inner MAX</t>
+  </si>
+  <si>
+    <t>Roundness_Inner Diameter</t>
+  </si>
+  <si>
+    <t>Roundness_Outer Diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter_Inner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter_Outer </t>
+  </si>
+  <si>
+    <t>Diameter_Outer  MIN</t>
+  </si>
+  <si>
+    <t>Diameter_Outer  MAX</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,39 +507,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>19</v>
@@ -571,37 +571,37 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -636,8 +636,8 @@
         <v>1.6717599999999999E-2</v>
       </c>
       <c r="K4" s="8">
-        <f>(J4/B4)*100</f>
-        <v>8.7758859132311517E-2</v>
+        <f>(J4/B4)*100/2</f>
+        <v>4.3879429566155759E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -672,8 +672,8 @@
         <v>2.2525199999999999E-2</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" ref="K5:K48" si="0">(J5/B5)*100</f>
-        <v>0.11837116024247517</v>
+        <f t="shared" ref="K5:K48" si="0">(J5/B5)*100/2</f>
+        <v>5.9185580121237584E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
       </c>
       <c r="K6" s="8">
         <f t="shared" si="0"/>
-        <v>7.2562934221216832E-2</v>
+        <v>3.6281467110608416E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
       </c>
       <c r="K7" s="8">
         <f t="shared" si="0"/>
-        <v>6.1271328341247391E-2</v>
+        <v>3.0635664170623696E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -781,7 +781,7 @@
       </c>
       <c r="K8" s="8">
         <f t="shared" si="0"/>
-        <v>4.6136045934806857E-2</v>
+        <v>2.3068022967403429E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -817,7 +817,7 @@
       </c>
       <c r="K9" s="8">
         <f t="shared" si="0"/>
-        <v>0.17031368586380735</v>
+        <v>8.5156842931903676E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
       </c>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>0.17182303489367884</v>
+        <v>8.5911517446839419E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -889,7 +889,7 @@
       </c>
       <c r="K11" s="8">
         <f t="shared" si="0"/>
-        <v>5.1221184870095138E-2</v>
+        <v>2.5610592435047569E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -925,7 +925,7 @@
       </c>
       <c r="K12" s="8">
         <f t="shared" si="0"/>
-        <v>0.17838156284857365</v>
+        <v>8.9190781424286825E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -961,7 +961,7 @@
       </c>
       <c r="K13" s="8">
         <f t="shared" si="0"/>
-        <v>0.16980301094519182</v>
+        <v>8.4901505472595909E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -997,7 +997,7 @@
       </c>
       <c r="K14" s="8">
         <f t="shared" si="0"/>
-        <v>0.16386537950968671</v>
+        <v>8.1932689754843357E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" si="0"/>
-        <v>0.14657664356698485</v>
+        <v>7.3288321783492427E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="K16" s="8">
         <f t="shared" si="0"/>
-        <v>0.15382243519071676</v>
+        <v>7.6911217595358378E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="K17" s="8">
         <f t="shared" si="0"/>
-        <v>0.17846860001582307</v>
+        <v>8.9234300007911535E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" si="0"/>
-        <v>0.14686708844192106</v>
+        <v>7.3433544220960531E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" si="0"/>
-        <v>0.16097082912294075</v>
+        <v>8.0485414561470375E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" si="0"/>
-        <v>8.3978741561488851E-2</v>
+        <v>4.1989370780744426E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="K21" s="8">
         <f t="shared" si="0"/>
-        <v>0.11355649944974121</v>
+        <v>5.6778249724870604E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" si="0"/>
-        <v>2.2240398605920347E-2</v>
+        <v>1.1120199302960173E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="K23" s="8">
         <f t="shared" si="0"/>
-        <v>0.18475248255353163</v>
+        <v>9.2376241276765816E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" si="0"/>
-        <v>1.8808853534852683E-2</v>
+        <v>9.4044267674263417E-3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" si="0"/>
-        <v>0.18208138045903238</v>
+        <v>9.1040690229516191E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" si="0"/>
-        <v>3.5170709259799267E-2</v>
+        <v>1.7585354629899633E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" si="0"/>
-        <v>0.18028426067265971</v>
+        <v>9.0142130336329854E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" si="0"/>
-        <v>0.1396424705630164</v>
+        <v>6.9821235281508201E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" si="0"/>
-        <v>1.0782638524930428E-2</v>
+        <v>5.3913192624652139E-3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" si="0"/>
-        <v>6.9015622435695825E-2</v>
+        <v>3.4507811217847913E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" si="0"/>
-        <v>0.19805000713704599</v>
+        <v>9.9025003568522993E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" si="0"/>
-        <v>9.4523842837092253E-2</v>
+        <v>4.7261921418546127E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" si="0"/>
-        <v>0.10388273405297699</v>
+        <v>5.1941367026488494E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" si="0"/>
-        <v>0.18069958071758588</v>
+        <v>9.0349790358792939E-2</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="0"/>
-        <v>0.14194159031115361</v>
+        <v>7.0970795155576805E-2</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" si="0"/>
-        <v>8.2393870553731902E-2</v>
+        <v>4.1196935276865951E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" si="0"/>
-        <v>0.1579232783688358</v>
+        <v>7.8961639184417898E-2</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" si="0"/>
-        <v>3.0874396691807107E-2</v>
+        <v>1.5437198345903553E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="K39" s="8">
         <f t="shared" si="0"/>
-        <v>3.500260624738824E-2</v>
+        <v>1.750130312369412E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="K40" s="8">
         <f t="shared" si="0"/>
-        <v>0.18474744401440299</v>
+        <v>9.2373722007201495E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="K41" s="8">
         <f t="shared" si="0"/>
-        <v>0.14208854609789356</v>
+        <v>7.1044273048946782E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="K42" s="8">
         <f t="shared" si="0"/>
-        <v>0.20516828445876048</v>
+        <v>0.10258414222938024</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="K43" s="8">
         <f t="shared" si="0"/>
-        <v>0.15859026323878991</v>
+        <v>7.9295131619394957E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="K44" s="8">
         <f t="shared" si="0"/>
-        <v>0.139648966682731</v>
+        <v>6.9824483341365498E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="K45" s="8">
         <f t="shared" si="0"/>
-        <v>0.16817530350567186</v>
+        <v>8.4087651752835932E-2</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="K46" s="8">
         <f t="shared" si="0"/>
-        <v>0.15664041576846291</v>
+        <v>7.8320207884231455E-2</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="K47" s="8">
         <f t="shared" si="0"/>
-        <v>0.18844054940140442</v>
+        <v>9.4220274700702211E-2</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2221,18 +2221,18 @@
       </c>
       <c r="K48" s="8">
         <f t="shared" si="0"/>
-        <v>4.1311896076117759E-2</v>
+        <v>2.0655948038058879E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4:E48 I4:J48">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="B4:D48 F4:H48">
+    <cfRule type="cellIs" dxfId="1" priority="39" operator="notBetween">
+      <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:D48 F4:H48">
-    <cfRule type="cellIs" dxfId="0" priority="39" operator="notBetween">
-      <formula>#REF!</formula>
+  <conditionalFormatting sqref="E4:E48 I4:J48">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>